<commit_message>
completed test cases, made initial revisions to design, and implemented code
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/PA1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leiflabianca/PycharmProjects/cs151-pa1-lelabianca/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0D32F8-6D7A-7B45-9670-B8699C8948C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E433D7-919C-4144-84FF-B56689E7FB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67920" windowHeight="28300" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,9 +34,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>You need to create your own tests</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+  <si>
+    <t>Selected clothing</t>
+  </si>
+  <si>
+    <t>Jacket</t>
+  </si>
+  <si>
+    <t>Pants</t>
+  </si>
+  <si>
+    <t>Scarf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable 1 (buttons, pockets, threads) </t>
+  </si>
+  <si>
+    <t>Win count</t>
+  </si>
+  <si>
+    <t>Variable 2 (thickness)</t>
+  </si>
+  <si>
+    <t>full win</t>
+  </si>
+  <si>
+    <t>half win</t>
+  </si>
+  <si>
+    <t>loss</t>
   </si>
 </sst>
 </file>
@@ -72,11 +99,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -95,9 +119,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -135,7 +159,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -241,7 +265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -383,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -391,27 +415,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF6E1F2-B43E-D343-BB9B-DE90F40B65C5}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="15" width="20.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>2.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0.1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0.99999990000000005</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>